<commit_message>
add lyrics for features
</commit_message>
<xml_diff>
--- a/data-raw/releases.xlsx
+++ b/data-raw/releases.xlsx
@@ -8,22 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakethompson/Documents/GIT/packages/taylor/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A102B33-B463-9E4E-94E1-A93274F62D6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1C78C78-A756-5F4A-86E6-D790C5FE8D02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21000" yWindow="-8060" windowWidth="21000" windowHeight="33100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="20160" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="releases" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">releases!$A$1:$D$93</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">releases!$A$1:$D$99</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="97">
   <si>
     <t>album_name</t>
   </si>
@@ -293,6 +293,27 @@
   </si>
   <si>
     <t>Mr. Perfectly Fine (Taylor's Version) [From The Vault]</t>
+  </si>
+  <si>
+    <t>Highway Don't Care</t>
+  </si>
+  <si>
+    <t>Babe</t>
+  </si>
+  <si>
+    <t>Two Is Better Than One</t>
+  </si>
+  <si>
+    <t>Half Of My Heart</t>
+  </si>
+  <si>
+    <t>Both Of Us</t>
+  </si>
+  <si>
+    <t>Gasoline (Remix)</t>
+  </si>
+  <si>
+    <t>Renegade</t>
   </si>
 </sst>
 </file>
@@ -1138,10 +1159,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D93"/>
+  <dimension ref="A1:D100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D94" sqref="D94"/>
+    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
+      <selection activeCell="A100" sqref="A100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1369,121 +1390,109 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>22</v>
+      <c r="B22" s="2" t="s">
+        <v>92</v>
       </c>
       <c r="D22" s="1">
-        <v>40112</v>
+        <v>40105</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" s="1">
+        <v>40112</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>12</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B24" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C24" s="1">
         <v>39735</v>
       </c>
-      <c r="D23" s="1">
+      <c r="D24" s="1">
         <v>40181</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B24" s="2" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B25" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D24" s="1">
+      <c r="D25" s="1">
         <v>40197</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>24</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D25" s="1">
-        <v>40394</v>
-      </c>
-    </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>24</v>
-      </c>
       <c r="B26" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C26" s="1">
-        <v>40455</v>
+        <v>93</v>
+      </c>
+      <c r="D26" s="1">
+        <v>40350</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>24</v>
       </c>
+      <c r="B27" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="D27" s="1">
-        <v>40476</v>
+        <v>40394</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>26</v>
-      </c>
-      <c r="D28" s="1">
-        <v>40476</v>
+        <v>24</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" s="1">
+        <v>40455</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>26</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C29" s="1">
-        <v>40490</v>
+        <v>24</v>
+      </c>
+      <c r="D29" s="1">
+        <v>40476</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C30" s="1">
-        <v>40490</v>
+      <c r="D30" s="1">
+        <v>40476</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>82</v>
+        <v>27</v>
       </c>
       <c r="C31" s="1">
-        <v>40462</v>
-      </c>
-      <c r="D31" s="1">
-        <v>40497</v>
+        <v>40490</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C32" s="1">
-        <v>40469</v>
-      </c>
-      <c r="D32" s="1">
-        <v>40615</v>
+        <v>40490</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
@@ -1491,10 +1500,13 @@
         <v>24</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
+      </c>
+      <c r="C33" s="1">
+        <v>40462</v>
       </c>
       <c r="D33" s="1">
-        <v>40652</v>
+        <v>40497</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -1502,70 +1514,70 @@
         <v>24</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
+      </c>
+      <c r="C34" s="1">
+        <v>40469</v>
       </c>
       <c r="D34" s="1">
-        <v>40742</v>
+        <v>40615</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
+        <v>24</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D35" s="1">
+        <v>40652</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>24</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D36" s="1">
+        <v>40742</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
         <v>26</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B37" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D35" s="1">
+      <c r="D37" s="1">
         <v>40869</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B36" s="2" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B38" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D36" s="1">
+      <c r="D38" s="1">
         <v>40903</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B37" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D37" s="1">
-        <v>40995</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>34</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D38" s="1">
-        <v>41134</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B39" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D39" s="1">
-        <v>41160</v>
+        <v>40995</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>34</v>
-      </c>
       <c r="B40" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C40" s="1">
-        <v>41177</v>
+        <v>94</v>
       </c>
       <c r="D40" s="1">
-        <v>41183</v>
+        <v>41051</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
@@ -1573,26 +1585,32 @@
         <v>34</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C41" s="1">
-        <v>41198</v>
+        <v>35</v>
+      </c>
+      <c r="D41" s="1">
+        <v>41134</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>34</v>
+      <c r="B42" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="D42" s="1">
-        <v>41204</v>
+        <v>41160</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>38</v>
+        <v>34</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C43" s="1">
+        <v>41177</v>
       </c>
       <c r="D43" s="1">
-        <v>41204</v>
+        <v>41183</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
@@ -1600,38 +1618,26 @@
         <v>34</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>39</v>
+        <v>84</v>
       </c>
       <c r="C44" s="1">
-        <v>41191</v>
-      </c>
-      <c r="D44" s="1">
-        <v>41253</v>
+        <v>41198</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>34</v>
       </c>
-      <c r="B45" s="2">
-        <v>22</v>
-      </c>
       <c r="D45" s="1">
-        <v>41345</v>
+        <v>41204</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>34</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C46" s="1">
-        <v>41184</v>
+        <v>38</v>
       </c>
       <c r="D46" s="1">
-        <v>41446</v>
+        <v>41204</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
@@ -1639,67 +1645,76 @@
         <v>34</v>
       </c>
       <c r="B47" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C47" s="1">
+        <v>41191</v>
+      </c>
+      <c r="D47" s="1">
+        <v>41253</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>34</v>
+      </c>
+      <c r="B48" s="2">
+        <v>22</v>
+      </c>
+      <c r="D48" s="1">
+        <v>41345</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B49" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D49" s="1">
+        <v>41358</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>34</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C50" s="1">
+        <v>41184</v>
+      </c>
+      <c r="D50" s="1">
+        <v>41446</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>34</v>
+      </c>
+      <c r="B51" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D47" s="1">
+      <c r="D51" s="1">
         <v>41471</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B48" s="2" t="s">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B52" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C48" s="1">
+      <c r="C52" s="1">
         <v>41568</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>34</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D49" s="1">
-        <v>41582</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50">
-        <v>1989</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D50" s="1">
-        <v>41869</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51">
-        <v>1989</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C51" s="1">
-        <v>41932</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52">
-        <v>1989</v>
-      </c>
-      <c r="D52" s="1">
-        <v>41939</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>45</v>
+        <v>34</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="D53" s="1">
-        <v>41939</v>
+        <v>41582</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
@@ -1707,10 +1722,10 @@
         <v>1989</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D54" s="1">
-        <v>41953</v>
+        <v>41869</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
@@ -1718,29 +1733,26 @@
         <v>1989</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D55" s="1">
-        <v>42044</v>
+        <v>44</v>
+      </c>
+      <c r="C55" s="1">
+        <v>41932</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B56" s="2" t="s">
-        <v>48</v>
+      <c r="A56">
+        <v>1989</v>
       </c>
       <c r="D56" s="1">
-        <v>42141</v>
+        <v>41939</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57">
-        <v>1989</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>49</v>
+      <c r="A57" t="s">
+        <v>45</v>
       </c>
       <c r="D57" s="1">
-        <v>42247</v>
+        <v>41939</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
@@ -1748,84 +1760,84 @@
         <v>1989</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C58" s="1">
-        <v>41926</v>
+        <v>46</v>
       </c>
       <c r="D58" s="1">
-        <v>42388</v>
+        <v>41953</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>45</v>
+      <c r="A59">
+        <v>1989</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D59" s="1">
-        <v>42423</v>
+        <v>42044</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B60" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D60" s="1">
-        <v>42713</v>
+        <v>42141</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>53</v>
+      <c r="A61">
+        <v>1989</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D61" s="1">
-        <v>42971</v>
+        <v>42247</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>53</v>
+      <c r="A62">
+        <v>1989</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C62" s="1">
-        <v>43028</v>
+        <v>41926</v>
+      </c>
+      <c r="D62" s="1">
+        <v>42388</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D63" s="1">
-        <v>43032</v>
+        <v>42423</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
-        <v>53</v>
-      </c>
       <c r="B64" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C64" s="1">
-        <v>43042</v>
+        <v>52</v>
+      </c>
+      <c r="D64" s="1">
+        <v>42713</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>53</v>
       </c>
+      <c r="B65" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="D65" s="1">
-        <v>43049</v>
+        <v>42971</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
@@ -1833,10 +1845,10 @@
         <v>53</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D66" s="1">
-        <v>43053</v>
+        <v>55</v>
+      </c>
+      <c r="C66" s="1">
+        <v>43028</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
@@ -1844,10 +1856,10 @@
         <v>53</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D67" s="1">
-        <v>43066</v>
+        <v>43032</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
@@ -1855,89 +1867,92 @@
         <v>53</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D68" s="1">
-        <v>43171</v>
+        <v>57</v>
+      </c>
+      <c r="C68" s="1">
+        <v>43042</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>53</v>
       </c>
-      <c r="B69" s="2" t="s">
-        <v>61</v>
-      </c>
       <c r="D69" s="1">
-        <v>43370</v>
+        <v>43049</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D70" s="1">
-        <v>43581</v>
+        <v>43053</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>85</v>
+        <v>59</v>
       </c>
       <c r="D71" s="1">
-        <v>43630</v>
+        <v>43066</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C72" s="1">
-        <v>43669</v>
+        <v>60</v>
+      </c>
+      <c r="D72" s="1">
+        <v>43171</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
-        <v>62</v>
-      </c>
       <c r="B73" s="2" t="s">
-        <v>62</v>
+        <v>91</v>
       </c>
       <c r="D73" s="1">
-        <v>43693</v>
+        <v>43210</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
+        <v>53</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D74" s="1">
+        <v>43370</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
         <v>62</v>
       </c>
-      <c r="D74" s="1">
-        <v>43700</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B75" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C75" s="1">
-        <v>43784</v>
+        <v>63</v>
+      </c>
+      <c r="D75" s="1">
+        <v>43581</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>62</v>
+      </c>
       <c r="B76" s="2" t="s">
-        <v>66</v>
+        <v>85</v>
       </c>
       <c r="D76" s="1">
-        <v>43805</v>
+        <v>43630</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
@@ -1945,172 +1960,234 @@
         <v>62</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D77" s="1">
-        <v>43857</v>
+        <v>64</v>
+      </c>
+      <c r="C77" s="1">
+        <v>43669</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>62</v>
+      </c>
       <c r="B78" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C78" s="1">
-        <v>43861</v>
+        <v>62</v>
+      </c>
+      <c r="D78" s="1">
+        <v>43693</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="D79" s="1">
-        <v>44036</v>
+        <v>43700</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
-        <v>70</v>
-      </c>
-      <c r="D80" s="1">
-        <v>44036</v>
+      <c r="B80" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C80" s="1">
+        <v>43784</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
-        <v>69</v>
-      </c>
       <c r="B81" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D81" s="1">
-        <v>44039</v>
+        <v>43805</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D82" s="1">
-        <v>44046</v>
+        <v>43857</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
-        <v>69</v>
-      </c>
       <c r="B83" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D83" s="1">
-        <v>44060</v>
+        <v>68</v>
+      </c>
+      <c r="C83" s="1">
+        <v>43861</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>69</v>
       </c>
-      <c r="B84" s="2" t="s">
-        <v>74</v>
-      </c>
       <c r="D84" s="1">
-        <v>44113</v>
+        <v>44036</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D85" s="1">
-        <v>44176</v>
+        <v>44036</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>76</v>
+        <v>69</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>71</v>
       </c>
       <c r="D86" s="1">
-        <v>44176</v>
+        <v>44039</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D87" s="1">
-        <v>44176</v>
+        <v>44046</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D88" s="1">
-        <v>44207</v>
+        <v>44060</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D89" s="1">
-        <v>44214</v>
+        <v>44113</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>80</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="D90" s="1">
-        <v>44239</v>
+        <v>44176</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>80</v>
-      </c>
-      <c r="B91" s="2" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="D91" s="1">
-        <v>44281</v>
+        <v>44176</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D92" s="1">
-        <v>44293</v>
+        <v>44176</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
+        <v>75</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D93" s="1">
+        <v>44207</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>75</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D94" s="1">
+        <v>44214</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
         <v>80</v>
       </c>
-      <c r="D93" s="1">
+      <c r="B95" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D95" s="1">
+        <v>44239</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B96" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D96" s="1">
+        <v>44246</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>80</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D97" s="1">
+        <v>44281</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>80</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D98" s="1">
+        <v>44293</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>80</v>
+      </c>
+      <c r="D99" s="1">
         <v>44295</v>
       </c>
     </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B100" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D100" s="1">
+        <v>44379</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:D93" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:D99" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add wildest dreams to releases
</commit_message>
<xml_diff>
--- a/data-raw/releases.xlsx
+++ b/data-raw/releases.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakethompson/Documents/GIT/packages/taylor/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDE25E25-A7B3-5E47-9BF1-67B687FF0103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55C167C0-2D50-264C-AFFC-D0CCFA3CF150}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="20160" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="99">
   <si>
     <t>album_name</t>
   </si>
@@ -317,6 +317,9 @@
   </si>
   <si>
     <t>Birch</t>
+  </si>
+  <si>
+    <t>Wildest Dreams (Taylor's Version)</t>
   </si>
 </sst>
 </file>
@@ -1162,10 +1165,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D101"/>
+  <dimension ref="A1:D102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="B102" sqref="B102"/>
+    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="C103" sqref="C103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2197,6 +2200,14 @@
         <v>44435</v>
       </c>
     </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B102" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C102" s="1">
+        <v>44456</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:D99" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
add spotify data for red (tv)
</commit_message>
<xml_diff>
--- a/data-raw/releases.xlsx
+++ b/data-raw/releases.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakethompson/Documents/GIT/packages/taylor/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55C167C0-2D50-264C-AFFC-D0CCFA3CF150}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF12CE39-0984-0C4F-9D52-56B4CA91E592}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="20160" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="100">
   <si>
     <t>album_name</t>
   </si>
@@ -320,6 +320,9 @@
   </si>
   <si>
     <t>Wildest Dreams (Taylor's Version)</t>
+  </si>
+  <si>
+    <t>Red (Taylor's Version)</t>
   </si>
 </sst>
 </file>
@@ -1165,10 +1168,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D102"/>
+  <dimension ref="A1:D103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
-      <selection activeCell="C103" sqref="C103"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="A104" sqref="A104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2208,6 +2211,14 @@
         <v>44456</v>
       </c>
     </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>99</v>
+      </c>
+      <c r="D103" s="1">
+        <v>44512</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:D99" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
this love (tv) + the joker and the queen
</commit_message>
<xml_diff>
--- a/data-raw/releases.xlsx
+++ b/data-raw/releases.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakethompson/Documents/GIT/packages/taylor/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF12CE39-0984-0C4F-9D52-56B4CA91E592}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02363DD4-56D8-CC4D-8C54-2C785805EC4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="20160" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="102">
   <si>
     <t>album_name</t>
   </si>
@@ -323,6 +323,12 @@
   </si>
   <si>
     <t>Red (Taylor's Version)</t>
+  </si>
+  <si>
+    <t>This Love (Taylor's Version)</t>
+  </si>
+  <si>
+    <t>The Joker And The Queen</t>
   </si>
 </sst>
 </file>
@@ -1168,10 +1174,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D103"/>
+  <dimension ref="A1:D105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="A104" sqref="A104"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="B103" sqref="B103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2212,11 +2218,27 @@
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A103" t="s">
+      <c r="B103" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C103" s="1">
+        <v>44498</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
         <v>99</v>
       </c>
-      <c r="D103" s="1">
+      <c r="D104" s="1">
         <v>44512</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B105" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C105" s="1">
+        <v>44687</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add carolina as single
</commit_message>
<xml_diff>
--- a/data-raw/releases.xlsx
+++ b/data-raw/releases.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakethompson/Documents/GIT/packages/taylor/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02363DD4-56D8-CC4D-8C54-2C785805EC4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E1219DC-766E-8349-AFF7-8AC38829F1AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="20160" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="103">
   <si>
     <t>album_name</t>
   </si>
@@ -329,6 +329,9 @@
   </si>
   <si>
     <t>The Joker And The Queen</t>
+  </si>
+  <si>
+    <t>Carolina</t>
   </si>
 </sst>
 </file>
@@ -1174,10 +1177,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D105"/>
+  <dimension ref="A1:D106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="B103" sqref="B103"/>
+    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="D106" sqref="D106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2213,32 +2216,40 @@
       <c r="B102" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C102" s="1">
+      <c r="D102" s="1">
         <v>44456</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B103" s="2" t="s">
+      <c r="A103" t="s">
+        <v>99</v>
+      </c>
+      <c r="D103" s="1">
+        <v>44512</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B104" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C103" s="1">
-        <v>44498</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A104" t="s">
-        <v>99</v>
-      </c>
       <c r="D104" s="1">
-        <v>44512</v>
+        <v>44603</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B105" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="C105" s="1">
+      <c r="D105" s="1">
         <v>44687</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B106" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D106" s="1">
+        <v>44736</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add lover-rmx, september, 3 sad virgins
</commit_message>
<xml_diff>
--- a/data-raw/releases.xlsx
+++ b/data-raw/releases.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakethompson/Documents/GIT/packages/taylor/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E1219DC-766E-8349-AFF7-8AC38829F1AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAA6E23E-DEF1-E24E-88D7-6BC03B7EFA5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="20160" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="releases" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">releases!$A$1:$D$99</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">releases!$A$1:$D$101</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="106">
   <si>
     <t>album_name</t>
   </si>
@@ -332,6 +332,15 @@
   </si>
   <si>
     <t>Carolina</t>
+  </si>
+  <si>
+    <t>September</t>
+  </si>
+  <si>
+    <t>Three Sad Virgins</t>
+  </si>
+  <si>
+    <t>Lover (Remix)</t>
   </si>
 </sst>
 </file>
@@ -1177,10 +1186,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D106"/>
+  <dimension ref="A1:D109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="D106" sqref="D106"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="B81" sqref="B81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1934,32 +1943,29 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B73" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D73" s="1">
+        <v>43203</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B74" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D73" s="1">
+      <c r="D74" s="1">
         <v>43210</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
-        <v>53</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D74" s="1">
-        <v>43370</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D75" s="1">
-        <v>43581</v>
+        <v>43370</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
@@ -1967,10 +1973,10 @@
         <v>62</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="D76" s="1">
-        <v>43630</v>
+        <v>43581</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
@@ -1978,10 +1984,10 @@
         <v>62</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C77" s="1">
-        <v>43669</v>
+        <v>85</v>
+      </c>
+      <c r="D77" s="1">
+        <v>43630</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
@@ -1989,91 +1995,88 @@
         <v>62</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D78" s="1">
-        <v>43693</v>
+        <v>64</v>
+      </c>
+      <c r="C78" s="1">
+        <v>43669</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>62</v>
       </c>
+      <c r="B79" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="D79" s="1">
+        <v>43693</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>62</v>
+      </c>
+      <c r="D80" s="1">
         <v>43700</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B80" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C80" s="1">
-        <v>43784</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B81" s="2" t="s">
-        <v>66</v>
+        <v>105</v>
       </c>
       <c r="D81" s="1">
-        <v>43805</v>
+        <v>43782</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
-        <v>62</v>
-      </c>
       <c r="B82" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D82" s="1">
-        <v>43857</v>
+        <v>65</v>
+      </c>
+      <c r="C82" s="1">
+        <v>43784</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B83" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C83" s="1">
-        <v>43861</v>
+        <v>66</v>
+      </c>
+      <c r="D83" s="1">
+        <v>43805</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>69</v>
+        <v>62</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="D84" s="1">
-        <v>44036</v>
+        <v>43857</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A85" t="s">
-        <v>70</v>
-      </c>
-      <c r="D85" s="1">
-        <v>44036</v>
+      <c r="B85" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C85" s="1">
+        <v>43861</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>69</v>
       </c>
-      <c r="B86" s="2" t="s">
-        <v>71</v>
-      </c>
       <c r="D86" s="1">
-        <v>44039</v>
+        <v>44036</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>69</v>
-      </c>
-      <c r="B87" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D87" s="1">
-        <v>44046</v>
+        <v>44036</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
@@ -2081,10 +2084,10 @@
         <v>69</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D88" s="1">
-        <v>44060</v>
+        <v>44039</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
@@ -2092,48 +2095,48 @@
         <v>69</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D89" s="1">
-        <v>44113</v>
+        <v>44046</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>75</v>
+        <v>69</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>73</v>
       </c>
       <c r="D90" s="1">
-        <v>44176</v>
+        <v>44060</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>76</v>
+        <v>69</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>74</v>
       </c>
       <c r="D91" s="1">
-        <v>44176</v>
+        <v>44113</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>75</v>
       </c>
-      <c r="B92" s="2" t="s">
-        <v>77</v>
-      </c>
       <c r="D92" s="1">
         <v>44176</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>75</v>
-      </c>
-      <c r="B93" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D93" s="1">
-        <v>44207</v>
+        <v>44176</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
@@ -2141,29 +2144,32 @@
         <v>75</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D94" s="1">
-        <v>44214</v>
+        <v>44176</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D95" s="1">
-        <v>44239</v>
+        <v>44207</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>75</v>
+      </c>
       <c r="B96" s="2" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="D96" s="1">
-        <v>44246</v>
+        <v>44214</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
@@ -2171,89 +2177,116 @@
         <v>80</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D97" s="1">
-        <v>44281</v>
+        <v>44239</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A98" t="s">
-        <v>80</v>
-      </c>
       <c r="B98" s="2" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="D98" s="1">
-        <v>44293</v>
+        <v>44246</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>80</v>
       </c>
+      <c r="B99" s="2" t="s">
+        <v>88</v>
+      </c>
       <c r="D99" s="1">
+        <v>44281</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>80</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D100" s="1">
+        <v>44293</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>80</v>
+      </c>
+      <c r="D101" s="1">
         <v>44295</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B100" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="D100" s="1">
-        <v>44379</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B101" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D101" s="1">
-        <v>44435</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B102" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D102" s="1">
-        <v>44456</v>
+        <v>44379</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A103" t="s">
-        <v>99</v>
+      <c r="B103" s="2" t="s">
+        <v>97</v>
       </c>
       <c r="D103" s="1">
-        <v>44512</v>
+        <v>44435</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B104" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D104" s="1">
-        <v>44603</v>
+        <v>44456</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B105" s="2" t="s">
-        <v>100</v>
+      <c r="A105" t="s">
+        <v>99</v>
       </c>
       <c r="D105" s="1">
-        <v>44687</v>
+        <v>44512</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B106" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D106" s="1">
+        <v>44513</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B107" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D107" s="1">
+        <v>44603</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B108" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D108" s="1">
+        <v>44687</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B109" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="D106" s="1">
+      <c r="D109" s="1">
         <v>44736</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D99" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:D101" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update single releases for midnights
</commit_message>
<xml_diff>
--- a/data-raw/releases.xlsx
+++ b/data-raw/releases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakethompson/Documents/GIT/packages/taylor/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40DFC3AF-3665-8443-BD01-C34D83121E2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44FE5FB2-99F4-B742-A24E-2D940A3880EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27120" yWindow="1220" windowWidth="27120" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="releases" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="117">
   <si>
     <t>album_name</t>
   </si>
@@ -368,6 +368,12 @@
   </si>
   <si>
     <t>Wonderland</t>
+  </si>
+  <si>
+    <t>Bejeweled</t>
+  </si>
+  <si>
+    <t>Question…?</t>
   </si>
 </sst>
 </file>
@@ -1215,10 +1221,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D118"/>
+  <dimension ref="A1:D120"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B82" sqref="B82:C82"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="A121" sqref="A121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2432,6 +2438,28 @@
         <v>44858</v>
       </c>
     </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>106</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C119" s="1">
+        <v>44859</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>106</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C120" s="1">
+        <v>44859</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:D102" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
add midnights til dawn edition tracks
</commit_message>
<xml_diff>
--- a/data-raw/releases.xlsx
+++ b/data-raw/releases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakethompson/Documents/GIT/packages/taylor/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F077CCA-7813-3F46-9602-68192B5585E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B68A9C2-B07D-6646-9B67-CDDF289E4251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="18980" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="125">
   <si>
     <t>album_name</t>
   </si>
@@ -395,6 +395,9 @@
   </si>
   <si>
     <t>Karma</t>
+  </si>
+  <si>
+    <t>Midnights (The Til Dawn Edition)</t>
   </si>
 </sst>
 </file>
@@ -1240,11 +1243,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D127"/>
+  <dimension ref="A1:D128"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A100" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A127" sqref="A127"/>
+      <pane ySplit="1" topLeftCell="A105" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A129" sqref="A129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2517,6 +2520,14 @@
         <v>45047</v>
       </c>
     </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>124</v>
+      </c>
+      <c r="D128" s="1">
+        <v>45072</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:D102" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
add lyrics to "You're Losing Me"
</commit_message>
<xml_diff>
--- a/data-raw/releases.xlsx
+++ b/data-raw/releases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakethompson/Documents/GIT/packages/taylor/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B68A9C2-B07D-6646-9B67-CDDF289E4251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C423D02-14E3-A943-A9E0-4D521F22F5EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="18980" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="126">
   <si>
     <t>album_name</t>
   </si>
@@ -398,6 +398,9 @@
   </si>
   <si>
     <t>Midnights (The Til Dawn Edition)</t>
+  </si>
+  <si>
+    <t>Midnights (The Late Night Edition)</t>
   </si>
 </sst>
 </file>
@@ -1243,11 +1246,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D128"/>
+  <dimension ref="A1:D129"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A105" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A129" sqref="A129"/>
+      <selection pane="bottomLeft" activeCell="A130" sqref="A130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2528,6 +2531,14 @@
         <v>45072</v>
       </c>
     </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>125</v>
+      </c>
+      <c r="D129" s="1">
+        <v>45072</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:D102" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
add cruel summer and sntv release dates
</commit_message>
<xml_diff>
--- a/data-raw/releases.xlsx
+++ b/data-raw/releases.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakethompson/Documents/GIT/packages/taylor/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C423D02-14E3-A943-A9E0-4D521F22F5EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD52E7FB-8FA1-7C4D-BB12-5F7F28F3E38C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="18980" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="128">
   <si>
     <t>album_name</t>
   </si>
@@ -401,6 +401,12 @@
   </si>
   <si>
     <t>Midnights (The Late Night Edition)</t>
+  </si>
+  <si>
+    <t>Cruel Summer</t>
+  </si>
+  <si>
+    <t>Speak Now (Taylor's Version)</t>
   </si>
 </sst>
 </file>
@@ -1246,11 +1252,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D129"/>
+  <dimension ref="A1:D131"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A105" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A130" sqref="A130"/>
+      <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A132" sqref="A132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2539,6 +2545,25 @@
         <v>45072</v>
       </c>
     </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>62</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D130" s="1">
+        <v>45097</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>127</v>
+      </c>
+      <c r="D131" s="1">
+        <v>45114</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:D102" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
move non-album singles to 1989 tv
</commit_message>
<xml_diff>
--- a/data-raw/releases.xlsx
+++ b/data-raw/releases.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakethompson/Documents/GIT/packages/taylor/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD52E7FB-8FA1-7C4D-BB12-5F7F28F3E38C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A047F3DA-86CE-1941-B891-AB297C090FAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="18980" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="129">
   <si>
     <t>album_name</t>
   </si>
@@ -407,6 +407,9 @@
   </si>
   <si>
     <t>Speak Now (Taylor's Version)</t>
+  </si>
+  <si>
+    <t>1989 (Taylor's Version)</t>
   </si>
 </sst>
 </file>
@@ -1252,11 +1255,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D131"/>
+  <dimension ref="A1:D132"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A132" sqref="A132"/>
+      <selection pane="bottomLeft" activeCell="B121" sqref="B121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2330,6 +2333,9 @@
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>128</v>
+      </c>
       <c r="B106" s="2" t="s">
         <v>98</v>
       </c>
@@ -2395,6 +2401,9 @@
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>128</v>
+      </c>
       <c r="B113" s="2" t="s">
         <v>100</v>
       </c>
@@ -2562,6 +2571,14 @@
       </c>
       <c r="D131" s="1">
         <v>45114</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>128</v>
+      </c>
+      <c r="D132" s="1">
+        <v>45226</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add 1989 tv data
</commit_message>
<xml_diff>
--- a/data-raw/releases.xlsx
+++ b/data-raw/releases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakethompson/Documents/GIT/packages/taylor/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A047F3DA-86CE-1941-B891-AB297C090FAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB8749CB-55B9-534A-BA69-215A0A717EBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="18980" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-31080" yWindow="1400" windowWidth="18980" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="releases" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="132">
   <si>
     <t>album_name</t>
   </si>
@@ -410,6 +410,15 @@
   </si>
   <si>
     <t>1989 (Taylor's Version)</t>
+  </si>
+  <si>
+    <t>1989 (Taylor's Version) [Deluxe]</t>
+  </si>
+  <si>
+    <t>1989 (Taylor's Version) [Tangerine Edition]</t>
+  </si>
+  <si>
+    <t>Slut! (Taylor's Version) [From The Vault]</t>
   </si>
 </sst>
 </file>
@@ -1255,16 +1264,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D132"/>
+  <dimension ref="A1:D135"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B121" sqref="B121"/>
+      <pane ySplit="1" topLeftCell="A103" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B136" sqref="B136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="46" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.1640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="15.33203125" style="1" customWidth="1"/>
@@ -2581,6 +2590,33 @@
         <v>45226</v>
       </c>
     </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>129</v>
+      </c>
+      <c r="D133" s="1">
+        <v>45226</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>130</v>
+      </c>
+      <c r="D134" s="1">
+        <v>45226</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>128</v>
+      </c>
+      <c r="B135" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C135" s="1">
+        <v>45226</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:D102" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
fix promo release date for "Slut!"
</commit_message>
<xml_diff>
--- a/data-raw/releases.xlsx
+++ b/data-raw/releases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakethompson/Documents/GIT/packages/taylor/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB8749CB-55B9-534A-BA69-215A0A717EBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85FCE30E-70D8-C04E-A197-AD44015791C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-31080" yWindow="1400" windowWidth="18980" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="releases" sheetId="1" r:id="rId1"/>
@@ -418,7 +418,7 @@
     <t>1989 (Taylor's Version) [Tangerine Edition]</t>
   </si>
   <si>
-    <t>Slut! (Taylor's Version) [From The Vault]</t>
+    <t>"Slut!" (Taylor's Version) [From The Vault]</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
add writing credit songs
</commit_message>
<xml_diff>
--- a/data-raw/releases.xlsx
+++ b/data-raw/releases.xlsx
@@ -1,29 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakethompson/Documents/GIT/packages/taylor/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49480D2A-0B18-C84E-96B9-05352CB2D263}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00D3D2B7-72B7-DC4B-A919-B95339245C6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35560" yWindow="600" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="19300" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="releases" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">releases!$A$1:$D$102</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">releases!$A$1:$D$108</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="145">
   <si>
     <t>album_name</t>
   </si>
@@ -434,6 +434,30 @@
   </si>
   <si>
     <t>Is It Over Now? (Taylor's Version) [From The Vault]</t>
+  </si>
+  <si>
+    <t>us.</t>
+  </si>
+  <si>
+    <t>1 step forward, 3 steps back</t>
+  </si>
+  <si>
+    <t>deja vu</t>
+  </si>
+  <si>
+    <t>Best Days Of Your Life</t>
+  </si>
+  <si>
+    <t>Better Man</t>
+  </si>
+  <si>
+    <t>This Is What You Came For</t>
+  </si>
+  <si>
+    <t>TMZ</t>
+  </si>
+  <si>
+    <t>You'll Always Find Your Way Back Home</t>
   </si>
 </sst>
 </file>
@@ -1279,11 +1303,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D140"/>
+  <dimension ref="A1:D148"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A108" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B137" sqref="B137"/>
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1459,44 +1483,38 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="B17" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D17" s="1">
+        <v>39783</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B18" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D18" s="1">
         <v>39789</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B18" s="2" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B19" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C19" s="1">
         <v>39892</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>12</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" s="1">
-        <v>39756</v>
-      </c>
-      <c r="D19" s="1">
-        <v>39921</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B20" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C20" s="1">
-        <v>39994</v>
+        <v>144</v>
+      </c>
+      <c r="D20" s="1">
+        <v>39896</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -1504,144 +1522,138 @@
         <v>12</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c r="C21" s="1">
+        <v>39756</v>
       </c>
       <c r="D21" s="1">
-        <v>40055</v>
+        <v>39921</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B22" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D22" s="1">
-        <v>40105</v>
+        <v>20</v>
+      </c>
+      <c r="C22" s="1">
+        <v>39994</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" s="1">
+        <v>40055</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B24" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D24" s="1">
+        <v>40105</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>22</v>
       </c>
-      <c r="D23" s="1">
+      <c r="D25" s="1">
         <v>40112</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>12</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B26" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C26" s="1">
         <v>39735</v>
       </c>
-      <c r="D24" s="1">
+      <c r="D26" s="1">
         <v>40181</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B25" s="2" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B27" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C27" s="1">
         <v>40197</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B26" s="2" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B28" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D26" s="1">
+      <c r="D28" s="1">
         <v>40350</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>24</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D27" s="1">
-        <v>40394</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>24</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C28" s="1">
-        <v>40455</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>24</v>
       </c>
+      <c r="B29" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="D29" s="1">
-        <v>40476</v>
+        <v>40394</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>26</v>
-      </c>
-      <c r="D30" s="1">
-        <v>40476</v>
+        <v>24</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C30" s="1">
+        <v>40455</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C31" s="1">
-        <v>40490</v>
+        <v>24</v>
+      </c>
+      <c r="D31" s="1">
+        <v>40476</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>26</v>
       </c>
-      <c r="B32" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C32" s="1">
-        <v>40490</v>
+      <c r="D32" s="1">
+        <v>40476</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>82</v>
+        <v>27</v>
       </c>
       <c r="C33" s="1">
-        <v>40462</v>
-      </c>
-      <c r="D33" s="1">
-        <v>40497</v>
+        <v>40490</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C34" s="1">
-        <v>40469</v>
-      </c>
-      <c r="D34" s="1">
-        <v>40615</v>
+        <v>40490</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -1649,10 +1661,13 @@
         <v>24</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
+      </c>
+      <c r="C35" s="1">
+        <v>40462</v>
       </c>
       <c r="D35" s="1">
-        <v>40652</v>
+        <v>40497</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
@@ -1660,78 +1675,78 @@
         <v>24</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
+      </c>
+      <c r="C36" s="1">
+        <v>40469</v>
       </c>
       <c r="D36" s="1">
-        <v>40742</v>
+        <v>40615</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>31</v>
+        <v>83</v>
       </c>
       <c r="D37" s="1">
-        <v>40869</v>
+        <v>40652</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B38" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D38" s="1">
+        <v>40715</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>24</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D39" s="1">
+        <v>40742</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>26</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D40" s="1">
+        <v>40869</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B41" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C38" s="1">
+      <c r="C41" s="1">
         <v>40903</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B39" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D39" s="1">
-        <v>40995</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B40" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D40" s="1">
-        <v>41051</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>34</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D41" s="1">
-        <v>41134</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B42" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D42" s="1">
-        <v>41160</v>
+        <v>40995</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>34</v>
-      </c>
       <c r="B43" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C43" s="1">
-        <v>41177</v>
+        <v>94</v>
       </c>
       <c r="D43" s="1">
-        <v>41183</v>
+        <v>41051</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
@@ -1739,26 +1754,32 @@
         <v>34</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C44" s="1">
-        <v>41198</v>
+        <v>35</v>
+      </c>
+      <c r="D44" s="1">
+        <v>41134</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>34</v>
+      <c r="B45" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="D45" s="1">
-        <v>41204</v>
+        <v>41160</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>38</v>
+        <v>34</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C46" s="1">
+        <v>41177</v>
       </c>
       <c r="D46" s="1">
-        <v>41204</v>
+        <v>41183</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
@@ -1766,32 +1787,26 @@
         <v>34</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>39</v>
+        <v>84</v>
       </c>
       <c r="C47" s="1">
-        <v>41191</v>
-      </c>
-      <c r="D47" s="1">
-        <v>41253</v>
+        <v>41198</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>34</v>
       </c>
-      <c r="B48" s="2">
-        <v>22</v>
-      </c>
       <c r="D48" s="1">
-        <v>41345</v>
+        <v>41204</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B49" s="2" t="s">
-        <v>90</v>
+      <c r="A49" t="s">
+        <v>38</v>
       </c>
       <c r="D49" s="1">
-        <v>41358</v>
+        <v>41204</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
@@ -1799,32 +1814,32 @@
         <v>34</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C50" s="1">
-        <v>41184</v>
+        <v>41191</v>
       </c>
       <c r="D50" s="1">
-        <v>41446</v>
+        <v>41253</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>34</v>
       </c>
-      <c r="B51" s="2" t="s">
-        <v>40</v>
+      <c r="B51" s="2">
+        <v>22</v>
       </c>
       <c r="D51" s="1">
-        <v>41471</v>
+        <v>41345</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B52" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C52" s="1">
-        <v>41568</v>
+        <v>90</v>
+      </c>
+      <c r="D52" s="1">
+        <v>41358</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
@@ -1832,48 +1847,54 @@
         <v>34</v>
       </c>
       <c r="B53" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C53" s="1">
+        <v>41184</v>
+      </c>
+      <c r="D53" s="1">
+        <v>41446</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>34</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D54" s="1">
+        <v>41471</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B55" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C55" s="1">
+        <v>41568</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>34</v>
+      </c>
+      <c r="B56" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D53" s="1">
+      <c r="D56" s="1">
         <v>41582</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57">
         <v>1989</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="B57" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D54" s="1">
+      <c r="D57" s="1">
         <v>41869</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55">
-        <v>1989</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C55" s="1">
-        <v>41932</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56">
-        <v>1989</v>
-      </c>
-      <c r="D56" s="1">
-        <v>41939</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>45</v>
-      </c>
-      <c r="D57" s="1">
-        <v>41939</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
@@ -1881,40 +1902,37 @@
         <v>1989</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D58" s="1">
-        <v>41953</v>
+        <v>44</v>
+      </c>
+      <c r="C58" s="1">
+        <v>41932</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>1989</v>
       </c>
-      <c r="B59" s="2" t="s">
-        <v>47</v>
-      </c>
       <c r="D59" s="1">
-        <v>42044</v>
+        <v>41939</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>45</v>
       </c>
-      <c r="B60" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C60" s="1">
-        <v>42052</v>
+      <c r="D60" s="1">
+        <v>41939</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>1989</v>
+      </c>
       <c r="B61" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D61" s="1">
-        <v>42141</v>
+        <v>41953</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
@@ -1922,98 +1940,92 @@
         <v>1989</v>
       </c>
       <c r="B62" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D62" s="1">
+        <v>42044</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>45</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C63" s="1">
+        <v>42052</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B64" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D64" s="1">
+        <v>42141</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>1989</v>
+      </c>
+      <c r="B65" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D62" s="1">
+      <c r="D65" s="1">
         <v>42247</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66">
         <v>1989</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="B66" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C63" s="1">
+      <c r="C66" s="1">
         <v>41926</v>
       </c>
-      <c r="D63" s="1">
+      <c r="D66" s="1">
         <v>42388</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
-        <v>45</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C64" s="1">
-        <v>42066</v>
-      </c>
-      <c r="D64" s="1">
-        <v>42423</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B65" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D65" s="1">
-        <v>42713</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>53</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D66" s="1">
-        <v>42971</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C67" s="1">
-        <v>43028</v>
+        <v>42066</v>
+      </c>
+      <c r="D67" s="1">
+        <v>42423</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
-        <v>53</v>
-      </c>
       <c r="B68" s="2" t="s">
-        <v>56</v>
+        <v>142</v>
       </c>
       <c r="D68" s="1">
-        <v>43032</v>
+        <v>42489</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
-        <v>53</v>
-      </c>
       <c r="B69" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C69" s="1">
-        <v>43042</v>
+        <v>141</v>
+      </c>
+      <c r="D69" s="1">
+        <v>42663</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
-        <v>53</v>
+      <c r="B70" s="2" t="s">
+        <v>52</v>
       </c>
       <c r="D70" s="1">
-        <v>43049</v>
+        <v>42713</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
@@ -2021,10 +2033,10 @@
         <v>53</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D71" s="1">
-        <v>43053</v>
+        <v>42971</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
@@ -2032,10 +2044,10 @@
         <v>53</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D72" s="1">
-        <v>43066</v>
+        <v>55</v>
+      </c>
+      <c r="C72" s="1">
+        <v>43028</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
@@ -2043,26 +2055,29 @@
         <v>53</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D73" s="1">
-        <v>43171</v>
+        <v>43032</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>53</v>
+      </c>
       <c r="B74" s="2" t="s">
-        <v>103</v>
+        <v>57</v>
       </c>
       <c r="C74" s="1">
-        <v>43203</v>
+        <v>43042</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B75" s="2" t="s">
-        <v>91</v>
+      <c r="A75" t="s">
+        <v>53</v>
       </c>
       <c r="D75" s="1">
-        <v>43210</v>
+        <v>43049</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
@@ -2070,86 +2085,92 @@
         <v>53</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D76" s="1">
-        <v>43370</v>
+        <v>43053</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D77" s="1">
-        <v>43581</v>
+        <v>43066</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>85</v>
+        <v>60</v>
       </c>
       <c r="D78" s="1">
-        <v>43630</v>
+        <v>43171</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
-        <v>62</v>
-      </c>
       <c r="B79" s="2" t="s">
-        <v>64</v>
+        <v>103</v>
       </c>
       <c r="C79" s="1">
-        <v>43669</v>
+        <v>43203</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
-        <v>62</v>
-      </c>
       <c r="B80" s="2" t="s">
-        <v>62</v>
+        <v>91</v>
       </c>
       <c r="D80" s="1">
-        <v>43693</v>
+        <v>43210</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
+        <v>53</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D81" s="1">
+        <v>43370</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
         <v>62</v>
       </c>
-      <c r="D81" s="1">
-        <v>43700</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B82" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="C82" s="1">
-        <v>43782</v>
+        <v>63</v>
+      </c>
+      <c r="D82" s="1">
+        <v>43581</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>62</v>
+      </c>
       <c r="B83" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C83" s="1">
-        <v>43784</v>
+        <v>85</v>
+      </c>
+      <c r="D83" s="1">
+        <v>43630</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>62</v>
+      </c>
       <c r="B84" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D84" s="1">
-        <v>43805</v>
+        <v>64</v>
+      </c>
+      <c r="C84" s="1">
+        <v>43669</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
@@ -2157,271 +2178,262 @@
         <v>62</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D85" s="1">
-        <v>43857</v>
+        <v>43693</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B86" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C86" s="1">
-        <v>43861</v>
+      <c r="A86" t="s">
+        <v>62</v>
+      </c>
+      <c r="D86" s="1">
+        <v>43700</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A87" t="s">
-        <v>69</v>
-      </c>
-      <c r="D87" s="1">
-        <v>44036</v>
+      <c r="B87" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C87" s="1">
+        <v>43782</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A88" t="s">
-        <v>70</v>
-      </c>
-      <c r="D88" s="1">
-        <v>44036</v>
+      <c r="B88" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C88" s="1">
+        <v>43784</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A89" t="s">
-        <v>69</v>
-      </c>
       <c r="B89" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D89" s="1">
-        <v>44039</v>
+        <v>43805</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D90" s="1">
-        <v>44046</v>
+        <v>43857</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A91" t="s">
-        <v>69</v>
-      </c>
       <c r="B91" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D91" s="1">
-        <v>44060</v>
+        <v>68</v>
+      </c>
+      <c r="C91" s="1">
+        <v>43861</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>69</v>
       </c>
-      <c r="B92" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C92" s="1">
-        <v>44113</v>
+      <c r="D92" s="1">
+        <v>44036</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D93" s="1">
-        <v>44176</v>
+        <v>44036</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>76</v>
+        <v>69</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>71</v>
       </c>
       <c r="D94" s="1">
-        <v>44176</v>
+        <v>44039</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D95" s="1">
-        <v>44176</v>
+        <v>44046</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D96" s="1">
-        <v>44207</v>
+        <v>44060</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D97" s="1">
-        <v>44214</v>
+        <v>74</v>
+      </c>
+      <c r="C97" s="1">
+        <v>44113</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>80</v>
-      </c>
-      <c r="B98" s="2" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="D98" s="1">
-        <v>44239</v>
+        <v>44176</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B99" s="2" t="s">
-        <v>95</v>
+      <c r="A99" t="s">
+        <v>76</v>
       </c>
       <c r="D99" s="1">
-        <v>44246</v>
+        <v>44176</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C100" s="1">
-        <v>44281</v>
+        <v>77</v>
+      </c>
+      <c r="D100" s="1">
+        <v>44176</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="C101" s="1">
-        <v>44293</v>
+        <v>78</v>
+      </c>
+      <c r="D101" s="1">
+        <v>44207</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
+        <v>75</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D102" s="1">
+        <v>44214</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
         <v>80</v>
       </c>
-      <c r="D102" s="1">
-        <v>44295</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B103" s="2" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="D103" s="1">
-        <v>44379</v>
+        <v>44239</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A104" t="s">
-        <v>70</v>
-      </c>
       <c r="B104" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="C104" s="1">
-        <v>44401</v>
+        <v>95</v>
+      </c>
+      <c r="D104" s="1">
+        <v>44246</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>80</v>
+      </c>
       <c r="B105" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D105" s="1">
-        <v>44435</v>
+        <v>88</v>
+      </c>
+      <c r="C105" s="1">
+        <v>44281</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A106" t="s">
-        <v>128</v>
-      </c>
       <c r="B106" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="C106" s="1">
-        <v>44456</v>
+        <v>139</v>
+      </c>
+      <c r="D106" s="1">
+        <v>44287</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>99</v>
-      </c>
-      <c r="D107" s="1">
-        <v>44512</v>
+        <v>80</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C107" s="1">
+        <v>44293</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>99</v>
-      </c>
-      <c r="B108" s="2" t="s">
-        <v>110</v>
+        <v>80</v>
       </c>
       <c r="D108" s="1">
-        <v>44512</v>
+        <v>44295</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B109" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C109" s="1">
-        <v>44513</v>
+        <v>138</v>
+      </c>
+      <c r="D109" s="1">
+        <v>44337</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A110" t="s">
-        <v>99</v>
-      </c>
       <c r="B110" s="2" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="D110" s="1">
-        <v>44515</v>
+        <v>44379</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>99</v>
+        <v>70</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C111" s="1">
-        <v>44515</v>
+        <v>44401</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B112" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D112" s="1">
-        <v>44603</v>
+        <v>44435</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
@@ -2429,126 +2441,132 @@
         <v>128</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C113" s="1">
-        <v>44687</v>
+        <v>44456</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B114" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="C114" s="1">
-        <v>44736</v>
+      <c r="A114" t="s">
+        <v>99</v>
+      </c>
+      <c r="D114" s="1">
+        <v>44512</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>106</v>
+        <v>99</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>110</v>
       </c>
       <c r="D115" s="1">
-        <v>44855</v>
+        <v>44512</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A116" t="s">
-        <v>107</v>
-      </c>
-      <c r="D116" s="1">
-        <v>44855</v>
+      <c r="B116" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C116" s="1">
+        <v>44513</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>108</v>
+        <v>99</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>109</v>
       </c>
       <c r="D117" s="1">
-        <v>44855</v>
+        <v>44515</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D118" s="1">
-        <v>44858</v>
+        <v>112</v>
+      </c>
+      <c r="C118" s="1">
+        <v>44515</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A119" t="s">
-        <v>106</v>
-      </c>
       <c r="B119" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="C119" s="1">
-        <v>44859</v>
+        <v>101</v>
+      </c>
+      <c r="D119" s="1">
+        <v>44603</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
+        <v>128</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C120" s="1">
+        <v>44687</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B121" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C121" s="1">
+        <v>44736</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
         <v>106</v>
       </c>
-      <c r="B120" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="C120" s="1">
+      <c r="D122" s="1">
+        <v>44855</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>107</v>
+      </c>
+      <c r="D123" s="1">
+        <v>44855</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>108</v>
+      </c>
+      <c r="D124" s="1">
+        <v>44855</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>106</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D125" s="1">
+        <v>44858</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>106</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C126" s="1">
         <v>44859</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A121" t="s">
-        <v>106</v>
-      </c>
-      <c r="B121" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="D121" s="1">
-        <v>44894</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B122" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="C122" s="1">
-        <v>45002</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B123" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="C123" s="1">
-        <v>45002</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B124" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="C124" s="1">
-        <v>45002</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B125" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="C125" s="1">
-        <v>45002</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B126" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="D126" s="1">
-        <v>45044</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
@@ -2556,133 +2574,203 @@
         <v>106</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="D127" s="1">
-        <v>45047</v>
+        <v>116</v>
+      </c>
+      <c r="C127" s="1">
+        <v>44859</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>124</v>
+        <v>106</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>117</v>
       </c>
       <c r="D128" s="1">
-        <v>45072</v>
+        <v>44894</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A129" t="s">
-        <v>125</v>
-      </c>
-      <c r="D129" s="1">
-        <v>45072</v>
+      <c r="B129" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C129" s="1">
+        <v>45002</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A130" t="s">
-        <v>62</v>
-      </c>
       <c r="B130" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="D130" s="1">
-        <v>45097</v>
+        <v>120</v>
+      </c>
+      <c r="C130" s="1">
+        <v>45002</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A131" t="s">
-        <v>127</v>
-      </c>
-      <c r="D131" s="1">
-        <v>45114</v>
+      <c r="B131" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C131" s="1">
+        <v>45002</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A132" t="s">
-        <v>128</v>
-      </c>
-      <c r="D132" s="1">
-        <v>45226</v>
+      <c r="B132" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C132" s="1">
+        <v>45002</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A133" t="s">
-        <v>129</v>
+      <c r="B133" s="2" t="s">
+        <v>118</v>
       </c>
       <c r="D133" s="1">
-        <v>45226</v>
+        <v>45044</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>130</v>
+        <v>106</v>
+      </c>
+      <c r="B134" s="2" t="s">
+        <v>123</v>
       </c>
       <c r="D134" s="1">
-        <v>45226</v>
+        <v>45047</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>128</v>
-      </c>
-      <c r="B135" s="2" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="D135" s="1">
-        <v>45226</v>
+        <v>45072</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>128</v>
-      </c>
-      <c r="B136" s="2" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="D136" s="1">
-        <v>45230</v>
+        <v>45072</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>125</v>
+        <v>62</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="C137" s="1">
-        <v>45259</v>
+        <v>126</v>
+      </c>
+      <c r="D137" s="1">
+        <v>45097</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D138" s="1">
-        <v>45401</v>
+        <v>45114</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="D139" s="1">
-        <v>45401</v>
+        <v>45226</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
+        <v>129</v>
+      </c>
+      <c r="D140" s="1">
+        <v>45226</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>130</v>
+      </c>
+      <c r="D141" s="1">
+        <v>45226</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>128</v>
+      </c>
+      <c r="B142" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D142" s="1">
+        <v>45226</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>128</v>
+      </c>
+      <c r="B143" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D143" s="1">
+        <v>45230</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>125</v>
+      </c>
+      <c r="B144" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C144" s="1">
+        <v>45259</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
         <v>132</v>
       </c>
-      <c r="B140" s="2" t="s">
+      <c r="D145" s="1">
+        <v>45401</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>133</v>
+      </c>
+      <c r="D146" s="1">
+        <v>45401</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
+        <v>132</v>
+      </c>
+      <c r="B147" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="D140" s="1">
+      <c r="D147" s="1">
         <v>45401</v>
       </c>
     </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B148" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D148" s="1">
+        <v>45464</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:D102" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:D108" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add icdiwabh single release
</commit_message>
<xml_diff>
--- a/data-raw/releases.xlsx
+++ b/data-raw/releases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakethompson/Documents/GIT/packages/taylor/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00D3D2B7-72B7-DC4B-A919-B95339245C6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{057A3613-E80F-CD4C-97D6-B706B6703D76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="19300" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="146">
   <si>
     <t>album_name</t>
   </si>
@@ -458,6 +458,9 @@
   </si>
   <si>
     <t>You'll Always Find Your Way Back Home</t>
+  </si>
+  <si>
+    <t>I Can Do It With A Broken Heart</t>
   </si>
 </sst>
 </file>
@@ -1303,11 +1306,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D148"/>
+  <dimension ref="A1:D149"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
+      <pane ySplit="1" topLeftCell="A133" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B149" sqref="B149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2769,6 +2772,17 @@
         <v>45464</v>
       </c>
     </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
+        <v>132</v>
+      </c>
+      <c r="B149" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D149" s="1">
+        <v>45475</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:D108" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>